<commit_message>
feat: refatoracao da aplicacao
</commit_message>
<xml_diff>
--- a/Planilhas/analise_ordinaria_consolidada.xlsx
+++ b/Planilhas/analise_ordinaria_consolidada.xlsx
@@ -6787,15 +6787,15 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>790357</v>
+        <v>792137</v>
       </c>
       <c r="B63" t="n">
-        <v>790357</v>
+        <v>792137</v>
       </c>
       <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr">
         <is>
-          <t>23 de Out de 2025</t>
+          <t>27 de Out de 2025</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -6810,7 +6810,7 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Art. 65, inciso II da Lei nº 13.445/2017; Art. 65, inciso IV da Lei nº 13.445/2017; Não anexou item 8; Não anexou item 3; Não anexou item 2</t>
+          <t>Art. 65, inciso II da Lei nº 13.445/2017</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
@@ -6845,22 +6845,22 @@
       </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>❌ NÃO ATENDIDO - Antecedentes criminais inválidos ou não anexados</t>
+          <t>✅ ATENDIDO</t>
         </is>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>✅ 25% (1/4)</t>
+          <t>✅ 100% (4/4)</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>3/8</t>
+          <t>7/8</t>
         </is>
       </c>
       <c r="Q63" t="inlineStr">
         <is>
-          <t>37.5%</t>
+          <t>87.5%</t>
         </is>
       </c>
       <c r="R63" t="inlineStr">
@@ -6870,113 +6870,10 @@
       </c>
       <c r="S63" t="inlineStr">
         <is>
-          <t>11:26:29</t>
+          <t>11:35:09</t>
         </is>
       </c>
       <c r="T63" t="inlineStr">
-        <is>
-          <t>Visando à instrução do processo de NATURALIZAÇÃO ORDINÁRIA requerido pelo Naturalizando MARCELDO ESTRAME, foram realizadas as diligências a seguir descritas:
-1. Não foi identificado início de falsidade documental ou contradição na documentação apresentada. 
-2. Para confirmação do tempo de residência por prazo indeterminado foram juntados ao processo:
-2.1. Certidão de Movimentos Migratórios
-2.1.1. O requerente NÃO ausentou-se do território nacional desde sua chegada em 2021 mas não foi registrad...</t>
-        </is>
-      </c>
-      <c r="U63" t="inlineStr">
-        <is>
-          <t>Não atendeu 2 requisito(s)</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>792137</v>
-      </c>
-      <c r="B64" t="n">
-        <v>792137</v>
-      </c>
-      <c r="C64" t="inlineStr"/>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>27 de Out de 2025</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>Naturalização Ordinária</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>Indeferimento</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>Art. 65, inciso II da Lei nº 13.445/2017</t>
-        </is>
-      </c>
-      <c r="H64" t="inlineStr">
-        <is>
-          <t>Indeferimento</t>
-        </is>
-      </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>Nenhum</t>
-        </is>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>Processo indeferido por não atender aos requisitos</t>
-        </is>
-      </c>
-      <c r="K64" t="inlineStr">
-        <is>
-          <t>✅ ATENDIDO</t>
-        </is>
-      </c>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>❌ NÃO ATENDIDO - Prazo de residência não localizado nos campos do sistema</t>
-        </is>
-      </c>
-      <c r="M64" t="inlineStr">
-        <is>
-          <t>✅ ATENDIDO</t>
-        </is>
-      </c>
-      <c r="N64" t="inlineStr">
-        <is>
-          <t>✅ ATENDIDO</t>
-        </is>
-      </c>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>✅ 100% (4/4)</t>
-        </is>
-      </c>
-      <c r="P64" t="inlineStr">
-        <is>
-          <t>7/8</t>
-        </is>
-      </c>
-      <c r="Q64" t="inlineStr">
-        <is>
-          <t>87.5%</t>
-        </is>
-      </c>
-      <c r="R64" t="inlineStr">
-        <is>
-          <t>16/11/2025</t>
-        </is>
-      </c>
-      <c r="S64" t="inlineStr">
-        <is>
-          <t>11:35:09</t>
-        </is>
-      </c>
-      <c r="T64" t="inlineStr">
         <is>
           <t>Assunto: Pedido de Naturalização ORDINÁRIA
 Processo: 792137
@@ -6987,109 +6884,101 @@
 3.	Em relação às condições exigidas para a naturalização ORDINÁRIA, verificou-se que a requerente possui autorização...</t>
         </is>
       </c>
-      <c r="U64" t="inlineStr">
+      <c r="U63" t="inlineStr">
         <is>
           <t>Não atendeu 1 requisito(s)</t>
         </is>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>790357</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>790357</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
+    <row r="64">
+      <c r="A64" t="n">
+        <v>790357</v>
+      </c>
+      <c r="B64" t="n">
+        <v>790357</v>
+      </c>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr">
         <is>
           <t>23 de Out de 2025</t>
         </is>
       </c>
-      <c r="E65" t="inlineStr">
+      <c r="E64" t="inlineStr">
         <is>
           <t>Naturalização Ordinária</t>
         </is>
       </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>Indeferimento</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Indeferimento</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
         <is>
           <t>Art. 65, inciso II da Lei nº 13.445/2017</t>
         </is>
       </c>
-      <c r="H65" t="inlineStr">
-        <is>
-          <t>Indeferimento</t>
-        </is>
-      </c>
-      <c r="I65" t="inlineStr">
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Indeferimento</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
         <is>
           <t>Nenhum</t>
         </is>
       </c>
-      <c r="J65" t="inlineStr">
+      <c r="J64" t="inlineStr">
         <is>
           <t>Processo indeferido por não atender aos requisitos</t>
         </is>
       </c>
-      <c r="K65" t="inlineStr">
-        <is>
-          <t>✅ ATENDIDO</t>
-        </is>
-      </c>
-      <c r="L65" t="inlineStr">
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
         <is>
           <t>❌ NÃO ATENDIDO - Prazo de residência não localizado nos campos do sistema</t>
         </is>
       </c>
-      <c r="M65" t="inlineStr">
-        <is>
-          <t>✅ ATENDIDO</t>
-        </is>
-      </c>
-      <c r="N65" t="inlineStr">
-        <is>
-          <t>✅ ATENDIDO</t>
-        </is>
-      </c>
-      <c r="O65" t="inlineStr">
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="O64" t="inlineStr">
         <is>
           <t>✅ 100% (4/4)</t>
         </is>
       </c>
-      <c r="P65" t="inlineStr">
+      <c r="P64" t="inlineStr">
         <is>
           <t>7/8</t>
         </is>
       </c>
-      <c r="Q65" t="inlineStr">
+      <c r="Q64" t="inlineStr">
         <is>
           <t>87.5%</t>
         </is>
       </c>
-      <c r="R65" t="inlineStr">
+      <c r="R64" t="inlineStr">
         <is>
           <t>16/11/2025</t>
         </is>
       </c>
-      <c r="S65" t="inlineStr">
+      <c r="S64" t="inlineStr">
         <is>
           <t>11:37:38</t>
         </is>
       </c>
-      <c r="T65" t="inlineStr">
+      <c r="T64" t="inlineStr">
         <is>
           <t>Visando à instrução do processo de NATURALIZAÇÃO ORDINÁRIA requerido pelo Naturalizando MARCELDO ESTRAME, foram realizadas as diligências a seguir descritas:
 1. Não foi identificado início de falsidade documental ou contradição na documentação apresentada. 
@@ -7098,9 +6987,119 @@
 2.1.1. O requerente NÃO ausentou-se do território nacional desde sua chegada em 2021 mas não foi registrad...</t>
         </is>
       </c>
+      <c r="U64" t="inlineStr">
+        <is>
+          <t>Não atendeu 1 requisito(s)</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>705567</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>705567</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>11 de Mar de 2025</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>Naturalização Ordinária</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Indeferimento</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>Art. 65, inciso II da Lei nº 13.445/2017; Art. 65, inciso III da Lei nº 13.445/2017; Art. 65, inciso IV da Lei nº 13.445/2017; Não anexou item 8; Não anexou item 4; Não anexou item 3; Não anexou item 2</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Indeferimento</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>Nenhum</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>Processo indeferido por não atender aos requisitos</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>❌ NÃO ATENDIDO - Prazo de residência não localizado nos campos do sistema</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>❌ NÃO ATENDIDO - Não anexou item 13 - Comprovante de comunicação em português</t>
+        </is>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>❌ NÃO ATENDIDO - Antecedentes criminais inválidos ou não anexados</t>
+        </is>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>✅ 0% (0/4)</t>
+        </is>
+      </c>
+      <c r="P65" t="inlineStr">
+        <is>
+          <t>1/8</t>
+        </is>
+      </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>12.5%</t>
+        </is>
+      </c>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>17/11/2025</t>
+        </is>
+      </c>
+      <c r="S65" t="inlineStr">
+        <is>
+          <t>13:35:18</t>
+        </is>
+      </c>
+      <c r="T65" t="inlineStr">
+        <is>
+          <t>1. Nos termos da legislação, realizadas as diligências necessárias à instrução do presente pedido de Transformação de Naturalização Provisória em Definitiva apresento o presente Relatório Opinativo.
+2. A relação de documentos exigidos pela legislação, foi apresentada integralmente conforme documentos juntados ao processo.
+3. De acordo com a documentação apresentada, o naturalizando possui capacidade civil.
+4. Em relação às condições exigidas para a transformação de naturalização provisória em...</t>
+        </is>
+      </c>
       <c r="U65" t="inlineStr">
         <is>
-          <t>Não atendeu 1 requisito(s)</t>
+          <t>Não atendeu 3 requisito(s)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualiza refatoracao do projeto
</commit_message>
<xml_diff>
--- a/Planilhas/analise_ordinaria_consolidada.xlsx
+++ b/Planilhas/analise_ordinaria_consolidada.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U65"/>
+  <dimension ref="A1:U71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6994,21 +6994,13 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>705567</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>705567</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>N/A</t>
-        </is>
-      </c>
+      <c r="A65" t="n">
+        <v>705567</v>
+      </c>
+      <c r="B65" t="n">
+        <v>705567</v>
+      </c>
+      <c r="C65" t="inlineStr"/>
       <c r="D65" t="inlineStr">
         <is>
           <t>11 de Mar de 2025</t>
@@ -7100,6 +7092,626 @@
       <c r="U65" t="inlineStr">
         <is>
           <t>Não atendeu 3 requisito(s)</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>768046</v>
+      </c>
+      <c r="B66" t="n">
+        <v>768046</v>
+      </c>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>1 de Set de 2025</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>Naturalização Ordinária</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Indeferimento</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>Art. 65, inciso II da Lei nº 13.445/2017; 🚨 REQUERENTE NÃO ESTÁ NO PAÍS - INDEFERIMENTO AUTOMÁTICO; Não anexou item 2</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Indeferimento</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>🚨 REQUERENTE NÃO ESTÁ NO PAÍS - INDEFERIMENTO AUTOMÁTICO</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>Processo indeferido por não atender aos requisitos</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>❌ NÃO ATENDIDO - Prazo de residência não localizado nos campos do sistema</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>✅ 75% (3/4)</t>
+        </is>
+      </c>
+      <c r="P66" t="inlineStr">
+        <is>
+          <t>6/8</t>
+        </is>
+      </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>75.0%</t>
+        </is>
+      </c>
+      <c r="R66" t="inlineStr">
+        <is>
+          <t>22/11/2025</t>
+        </is>
+      </c>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>14:36:14</t>
+        </is>
+      </c>
+      <c r="T66" t="inlineStr">
+        <is>
+          <t>1. Nos termos da legislação, realizadas as diligências necessárias à instrução do presente pedido de Naturalização Ordinária apresento o presente Relatório Opinativo.
+2. Conforme registro no Sistema de Tráfego Internacional - STI e no passaporte, o requerente não se encontra em território nacional na data da entrada do processo, impedindo a continuidade do processo.
+3. Diante do exposto, encaminhe-se ao Ministério da Justiça e Segurança Pública com opinião DESFAVORÁVEL AO DEFERIMENTO em razão ...</t>
+        </is>
+      </c>
+      <c r="U66" t="inlineStr">
+        <is>
+          <t>Não atendeu 2 requisito(s)</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>767995</v>
+      </c>
+      <c r="B67" t="n">
+        <v>767995</v>
+      </c>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>1 de Set de 2025</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>Naturalização Ordinária</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Indeferimento</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>⚠️ AUSÊNCIA DE COLETA BIOMÉTRICA CONSTATADA NO PARECER PF</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Indeferimento</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>⚠️ AUSÊNCIA DE COLETA BIOMÉTRICA CONSTATADA NO PARECER PF</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>Processo indeferido por não atender aos requisitos</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>✅ 100% (4/4)</t>
+        </is>
+      </c>
+      <c r="P67" t="inlineStr">
+        <is>
+          <t>8/8</t>
+        </is>
+      </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="R67" t="inlineStr">
+        <is>
+          <t>22/11/2025</t>
+        </is>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>14:38:42</t>
+        </is>
+      </c>
+      <c r="T67" t="inlineStr">
+        <is>
+          <t>1.	Nos termos da legislação, realizadas as diligências necessárias à instrução do presente pedido de Naturalização Ordinária apresento o presente Relatório Opinativo.
+2.	De acordo com a documentação apresentada, o interessado possui capacidade civil. 
+3.	A relação de documentos exigidos pela legislação, NÃO foi apresentada integralmente conforme documentos juntados ao processo. NÃO apresentou:
+a.	Legalização ou apostilamento do atestado de antecedentes criminais emitido pelo país de origem (o do...</t>
+        </is>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
+          <t>Não atendeu 1 requisito(s)</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>767111</v>
+      </c>
+      <c r="B68" t="n">
+        <v>767111</v>
+      </c>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>29 de Ago de 2025</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>Naturalização Ordinária</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Analise Manual</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Art. 65, inciso II da Lei nº 13.445/2017</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Indeferimento</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>⚠️ PARECER PF SEM PRAZO DE RESIDÊNCIA ESPECIFICADO</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>Processo encaminhado para ANÁLISE MANUAL devido a alerta(s) crítico(s) no parecer da PF ou dados insuficientes para decisão automática.</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>❌ NÃO ATENDIDO - Tempo insuficiente: 1.00 anos &lt; 3.95 anos</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>✅ 100% (4/4)</t>
+        </is>
+      </c>
+      <c r="P68" t="inlineStr">
+        <is>
+          <t>7/8</t>
+        </is>
+      </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>87.5%</t>
+        </is>
+      </c>
+      <c r="R68" t="inlineStr">
+        <is>
+          <t>22/11/2025</t>
+        </is>
+      </c>
+      <c r="S68" t="inlineStr">
+        <is>
+          <t>14:40:59</t>
+        </is>
+      </c>
+      <c r="T68" t="inlineStr">
+        <is>
+          <t>Nos termos da legislação, realizadas as diligências necessárias à instrução do presente pedido de naturalização, apresento o presente Relatório Opinativo. 
+O artigo 65 da Lei 13.445/17 estabelece os seguintes requisitos para o deferimento da naturalização ordinária:
+I - ter capacidade civil, segundo a lei brasileira;
+II - ter residência em território nacional, pelo prazo mínimo de 4 (quatro) anos;
+III - comunicar-se em língua portuguesa, consideradas as condições do naturalizando; e
+IV - nã...</t>
+        </is>
+      </c>
+      <c r="U68" t="inlineStr">
+        <is>
+          <t>Caso marcado para análise manual (sem decisão automática de deferimento/indeferimento).</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>765992</v>
+      </c>
+      <c r="B69" t="n">
+        <v>765992</v>
+      </c>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>27 de Ago de 2025</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>Naturalização Ordinária</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Deferimento</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Indeferimento</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>Nenhum</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>Processo deferido automaticamente com base na análise de elegibilidade.</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>✅ 100% (4/4)</t>
+        </is>
+      </c>
+      <c r="P69" t="inlineStr">
+        <is>
+          <t>8/8</t>
+        </is>
+      </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="R69" t="inlineStr">
+        <is>
+          <t>22/11/2025</t>
+        </is>
+      </c>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>14:44:28</t>
+        </is>
+      </c>
+      <c r="T69" t="inlineStr">
+        <is>
+          <t>RELATóRIO OPINATIVO/PARECER
+DATA 08/09/2025
+Naturalizando
+MOISE STERLING - G2975982: 
+1. Nos termos da legislação, realizadas as diligências necessárias à instrução do presente pedido de Naturalização Ordinária apresento o presente Relatório Opinativo/Parecer.
+2. A relação de documentos exigidos pela legislação, não foi apresentada integralmente conforme documentos juntados ao processo, visto que o naturalizando não compareceu nem justificou a falta ao agendamento/notificação.
+3. Notific...</t>
+        </is>
+      </c>
+      <c r="U69" t="inlineStr">
+        <is>
+          <t>Todos os requisitos atendidos segundo a análise automática.</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>763365</v>
+      </c>
+      <c r="B70" t="n">
+        <v>763365</v>
+      </c>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>20 de Ago de 2025</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>Naturalização Ordinária</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Deferimento</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Indeferimento</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>Nenhum</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>Processo deferido automaticamente com base na análise de elegibilidade.</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>✅ 100% (4/4)</t>
+        </is>
+      </c>
+      <c r="P70" t="inlineStr">
+        <is>
+          <t>8/8</t>
+        </is>
+      </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>100.0%</t>
+        </is>
+      </c>
+      <c r="R70" t="inlineStr">
+        <is>
+          <t>22/11/2025</t>
+        </is>
+      </c>
+      <c r="S70" t="inlineStr">
+        <is>
+          <t>14:46:23</t>
+        </is>
+      </c>
+      <c r="T70" t="inlineStr">
+        <is>
+          <t>RELATóRIO OPINATIVO/PARECER
+DATA 29/08/2025
+Naturalizando
+JAMESLEY ESTIMABLE - G314924Y: 
+1. Nos termos da legislação, realizadas as diligências necessárias à instrução do presente pedido de Naturalização Ordinária apresento o presente Relatório Opinativo/Parecer.
+2. A relação de documentos exigidos pela legislação, não foi apresentada integralmente conforme documentos juntados ao processo, visto que o naturalizando não compareceu nem justificou a falta ao agendamento/notificação.
+3. Not...</t>
+        </is>
+      </c>
+      <c r="U70" t="inlineStr">
+        <is>
+          <t>Todos os requisitos atendidos segundo a análise automática.</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>762641</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>762641</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>18 de Ago de 2025</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>Naturalização Ordinária</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Indeferimento</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Art. 65, inciso IV da Lei nº 13.445/2017; ⚠️ AUSÊNCIA DE COLETA BIOMÉTRICA CONSTATADA NO PARECER PF; Não anexou item 4</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Indeferimento</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>⚠️ AUSÊNCIA DE COLETA BIOMÉTRICA CONSTATADA NO PARECER PF</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>Processo indeferido por não atender aos requisitos</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>✅ ATENDIDO</t>
+        </is>
+      </c>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>❌ NÃO ATENDIDO - Antecedentes criminais inválidos ou não anexados</t>
+        </is>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>✅ 75% (3/4)</t>
+        </is>
+      </c>
+      <c r="P71" t="inlineStr">
+        <is>
+          <t>6/8</t>
+        </is>
+      </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>75.0%</t>
+        </is>
+      </c>
+      <c r="R71" t="inlineStr">
+        <is>
+          <t>22/11/2025</t>
+        </is>
+      </c>
+      <c r="S71" t="inlineStr">
+        <is>
+          <t>14:47:25</t>
+        </is>
+      </c>
+      <c r="T71" t="inlineStr">
+        <is>
+          <t>1.	Nos termos da legislação, realizadas as diligências necessárias à instrução do presente pedido de Naturalização Ordinária apresento o presente Relatório Opinativo.
+2.	De acordo com a documentação apresentada, o interessado possui capacidade civil. 
+3.	A relação de documentos exigidos pela legislação, NÃO foi apresentada integralmente conforme documentos juntados ao processo. NÃO apresentou:
+a.	Cópia da Carteira de Registro Nacional Migratório;
+b.	Comprovante de situação cadastral do Cadastro ...</t>
+        </is>
+      </c>
+      <c r="U71" t="inlineStr">
+        <is>
+          <t>Não atendeu 2 requisito(s)</t>
         </is>
       </c>
     </row>

</xml_diff>